<commit_message>
Fixed database connectivity and API endpoints
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zatar\PycharmProjects\PythonProject11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DE9617-377B-48DB-B950-7F9716737C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47FFB8D-EDFC-43B1-8EA5-BCB87821C4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D8B9CE04-17E9-4983-9B8C-CAEE159B15CD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="125">
   <si>
     <t>name</t>
   </si>
@@ -402,6 +402,15 @@
   </si>
   <si>
     <t>PD0325701</t>
+  </si>
+  <si>
+    <t>hEGF</t>
+  </si>
+  <si>
+    <t>E9644-.5MG</t>
+  </si>
+  <si>
+    <t>https://www.sigmaaldrich.com/MX/es/product/sigma/e9644?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=22179178721&amp;utm_content=177793360441&amp;gad_source=1&amp;gad_campaignid=22179178721&amp;gbraid=0AAAAAD8kLQQijHqI3ftWe1h-KzX0veMTN&amp;gclid=CjwKCAjwtfvEBhAmEiwA-DsKjncC52MuEisnbBttGKNLUW_jnD-jpKIWAwJoS3ZTUteNgQdjhKakFxoCKgUQAvD_BwE</t>
   </si>
 </sst>
 </file>
@@ -779,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E216E284-F5CA-4C13-9ED2-87D2CAE05C0A}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2133,6 +2142,41 @@
         <v>40</v>
       </c>
     </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>122</v>
+      </c>
+      <c r="C41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D41" t="s">
+        <v>124</v>
+      </c>
+      <c r="E41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F41" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41">
+        <v>-30</v>
+      </c>
+      <c r="H41">
+        <v>9</v>
+      </c>
+      <c r="I41" t="s">
+        <v>55</v>
+      </c>
+      <c r="J41">
+        <v>52</v>
+      </c>
+      <c r="K41" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
UPDATE: Inventory quantity adjustments and history tracking
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zatar\PycharmProjects\PythonProject11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47FFB8D-EDFC-43B1-8EA5-BCB87821C4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181AD262-705C-4B36-8379-F0FADD92EA9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D8B9CE04-17E9-4983-9B8C-CAEE159B15CD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="131">
   <si>
     <t>name</t>
   </si>
@@ -411,6 +411,24 @@
   </si>
   <si>
     <t>https://www.sigmaaldrich.com/MX/es/product/sigma/e9644?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=22179178721&amp;utm_content=177793360441&amp;gad_source=1&amp;gad_campaignid=22179178721&amp;gbraid=0AAAAAD8kLQQijHqI3ftWe1h-KzX0veMTN&amp;gclid=CjwKCAjwtfvEBhAmEiwA-DsKjncC52MuEisnbBttGKNLUW_jnD-jpKIWAwJoS3ZTUteNgQdjhKakFxoCKgUQAvD_BwE</t>
+  </si>
+  <si>
+    <t>Y27632</t>
+  </si>
+  <si>
+    <t>70 uL</t>
+  </si>
+  <si>
+    <t>E8 Supplement</t>
+  </si>
+  <si>
+    <t>A1517-01</t>
+  </si>
+  <si>
+    <t>https://www.stemcell.com/products/y-27632.html</t>
+  </si>
+  <si>
+    <t>https://www.thermofisher.com/order/catalog/product/A1517001</t>
   </si>
 </sst>
 </file>
@@ -788,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E216E284-F5CA-4C13-9ED2-87D2CAE05C0A}">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="M45" sqref="M45"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2177,6 +2195,76 @@
         <v>38</v>
       </c>
     </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42">
+        <v>72304</v>
+      </c>
+      <c r="D42" t="s">
+        <v>129</v>
+      </c>
+      <c r="E42" t="s">
+        <v>32</v>
+      </c>
+      <c r="F42" t="s">
+        <v>19</v>
+      </c>
+      <c r="G42">
+        <v>-30</v>
+      </c>
+      <c r="H42">
+        <v>9</v>
+      </c>
+      <c r="I42" t="s">
+        <v>55</v>
+      </c>
+      <c r="J42">
+        <v>60</v>
+      </c>
+      <c r="K42" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>127</v>
+      </c>
+      <c r="C43" t="s">
+        <v>128</v>
+      </c>
+      <c r="D43" t="s">
+        <v>130</v>
+      </c>
+      <c r="E43" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" t="s">
+        <v>19</v>
+      </c>
+      <c r="G43">
+        <v>-30</v>
+      </c>
+      <c r="H43">
+        <v>9</v>
+      </c>
+      <c r="I43" t="s">
+        <v>55</v>
+      </c>
+      <c r="J43">
+        <v>11</v>
+      </c>
+      <c r="K43" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add persistent database support for Render
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zatar\PycharmProjects\PythonProject11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181AD262-705C-4B36-8379-F0FADD92EA9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC377B1-C507-477F-BF5B-AFB244DC0EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D8B9CE04-17E9-4983-9B8C-CAEE159B15CD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="139">
   <si>
     <t>name</t>
   </si>
@@ -429,6 +429,30 @@
   </si>
   <si>
     <t>https://www.thermofisher.com/order/catalog/product/A1517001</t>
+  </si>
+  <si>
+    <t>Human Fibronectin</t>
+  </si>
+  <si>
+    <t>Matrix</t>
+  </si>
+  <si>
+    <t>Refri cultivo</t>
+  </si>
+  <si>
+    <t>1 mg</t>
+  </si>
+  <si>
+    <t>https://ecatalog.corning.com/life-sciences/b2b/MX/en/Surfaces/Extracellular-Matrices-ECMs/Corning%C2%AE-Fibronectin/p/354008</t>
+  </si>
+  <si>
+    <t>BMS493</t>
+  </si>
+  <si>
+    <t>50 uL, 5mM</t>
+  </si>
+  <si>
+    <t>https://www.medchemexpress.com/bms493.html?utm_source=google&amp;utm_medium=CPC&amp;utm_campaign=US&amp;utm_term=BMS493&amp;utm_content=BMS493&amp;gad_source=1&amp;gad_campaignid=1725972650&amp;gbraid=0AAAAADnIT_ZkQaOPETcPVScp9AY3-4w_B&amp;gclid=CjwKCAjwq9rFBhAIEiwAGVAZP8w4pNg7K_ExIznm_tWhkcKCW6IzFowqlST_89LXwdrE2aKS1RJLnBoC_mYQAvD_BwE</t>
   </si>
 </sst>
 </file>
@@ -470,8 +494,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -806,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E216E284-F5CA-4C13-9ED2-87D2CAE05C0A}">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2265,6 +2290,70 @@
         <v>38</v>
       </c>
     </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>131</v>
+      </c>
+      <c r="C44">
+        <v>354008</v>
+      </c>
+      <c r="D44" t="s">
+        <v>135</v>
+      </c>
+      <c r="E44" t="s">
+        <v>132</v>
+      </c>
+      <c r="F44" t="s">
+        <v>15</v>
+      </c>
+      <c r="G44" t="s">
+        <v>133</v>
+      </c>
+      <c r="I44" t="s">
+        <v>14</v>
+      </c>
+      <c r="J44">
+        <v>3</v>
+      </c>
+      <c r="K44" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>136</v>
+      </c>
+      <c r="C45" s="1">
+        <v>411937</v>
+      </c>
+      <c r="D45" t="s">
+        <v>138</v>
+      </c>
+      <c r="E45" t="s">
+        <v>32</v>
+      </c>
+      <c r="F45" t="s">
+        <v>19</v>
+      </c>
+      <c r="G45" t="s">
+        <v>133</v>
+      </c>
+      <c r="I45" t="s">
+        <v>55</v>
+      </c>
+      <c r="J45">
+        <v>64</v>
+      </c>
+      <c r="K45" t="s">
+        <v>137</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>